<commit_message>
Updated data analysis notebook and documents
</commit_message>
<xml_diff>
--- a/data_analysis/task_1_2.xlsx
+++ b/data_analysis/task_1_2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF17E83-E700-4073-B801-9646FC56DE2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4740FB18-4E8C-4ED3-80B5-F8134AF70D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="3240" windowWidth="33870" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23955" yWindow="3765" windowWidth="24480" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks1&amp;2" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="38">
   <si>
     <t>Group</t>
   </si>
@@ -127,6 +127,24 @@
   </si>
   <si>
     <t>COG_TOT</t>
+  </si>
+  <si>
+    <t>LOC_PROD</t>
+  </si>
+  <si>
+    <t>LOC_TEST</t>
+  </si>
+  <si>
+    <t>LOC_TOT</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
   </si>
 </sst>
 </file>
@@ -537,19 +555,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomLeft" activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="15" width="10.7109375" customWidth="1"/>
+    <col min="1" max="21" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -595,8 +613,26 @@
       <c r="O1" s="7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -644,8 +680,26 @@
         <f t="shared" ref="O2:O19" si="1">SUM(M2:N2)</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" s="8">
+        <v>102</v>
+      </c>
+      <c r="Q2" s="8">
+        <v>60</v>
+      </c>
+      <c r="R2" s="8">
+        <v>162</v>
+      </c>
+      <c r="S2" s="8">
+        <v>5</v>
+      </c>
+      <c r="T2" s="8">
+        <v>3</v>
+      </c>
+      <c r="U2" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -693,8 +747,26 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3" s="8">
+        <v>146</v>
+      </c>
+      <c r="Q3" s="8">
+        <v>81</v>
+      </c>
+      <c r="R3" s="8">
+        <v>207</v>
+      </c>
+      <c r="S3" s="8">
+        <v>3</v>
+      </c>
+      <c r="T3" s="8">
+        <v>3</v>
+      </c>
+      <c r="U3" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -742,8 +814,26 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4" s="8">
+        <v>90</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>64</v>
+      </c>
+      <c r="R4" s="8">
+        <v>154</v>
+      </c>
+      <c r="S4" s="8">
+        <v>4</v>
+      </c>
+      <c r="T4" s="8">
+        <v>2</v>
+      </c>
+      <c r="U4" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -791,8 +881,26 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" s="8">
+        <v>121</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>57</v>
+      </c>
+      <c r="R5" s="8">
+        <v>178</v>
+      </c>
+      <c r="S5" s="8">
+        <v>4</v>
+      </c>
+      <c r="T5" s="8">
+        <v>3</v>
+      </c>
+      <c r="U5" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -840,8 +948,26 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6" s="8">
+        <v>93</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>102</v>
+      </c>
+      <c r="R6" s="8">
+        <v>195</v>
+      </c>
+      <c r="S6" s="8">
+        <v>5</v>
+      </c>
+      <c r="T6" s="8">
+        <v>4</v>
+      </c>
+      <c r="U6" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -889,8 +1015,26 @@
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7" s="8">
+        <v>164</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>96</v>
+      </c>
+      <c r="R7" s="8">
+        <v>260</v>
+      </c>
+      <c r="S7" s="8">
+        <v>5</v>
+      </c>
+      <c r="T7" s="8">
+        <v>3</v>
+      </c>
+      <c r="U7" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -938,8 +1082,26 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8" s="8">
+        <v>90</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>67</v>
+      </c>
+      <c r="R8" s="8">
+        <v>157</v>
+      </c>
+      <c r="S8" s="8">
+        <v>3</v>
+      </c>
+      <c r="T8" s="8">
+        <v>3</v>
+      </c>
+      <c r="U8" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
@@ -987,8 +1149,26 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9" s="8">
+        <v>111</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>74</v>
+      </c>
+      <c r="R9" s="8">
+        <v>185</v>
+      </c>
+      <c r="S9" s="8">
+        <v>4</v>
+      </c>
+      <c r="T9" s="8">
+        <v>3</v>
+      </c>
+      <c r="U9" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1036,8 +1216,26 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10" s="8">
+        <v>82</v>
+      </c>
+      <c r="Q10" s="8">
+        <v>8</v>
+      </c>
+      <c r="R10" s="8">
+        <v>100</v>
+      </c>
+      <c r="S10" s="8">
+        <v>4</v>
+      </c>
+      <c r="T10" s="8">
+        <v>3</v>
+      </c>
+      <c r="U10" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1085,8 +1283,26 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11" s="8">
+        <v>86</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>27</v>
+      </c>
+      <c r="R11" s="8">
+        <v>113</v>
+      </c>
+      <c r="S11" s="8">
+        <v>2</v>
+      </c>
+      <c r="T11" s="8">
+        <v>2</v>
+      </c>
+      <c r="U11" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
@@ -1134,8 +1350,26 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P12" s="8">
+        <v>90</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>45</v>
+      </c>
+      <c r="R12" s="8">
+        <v>135</v>
+      </c>
+      <c r="S12" s="8">
+        <v>5</v>
+      </c>
+      <c r="T12" s="8">
+        <v>4</v>
+      </c>
+      <c r="U12" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
@@ -1183,8 +1417,26 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P13" s="8">
+        <v>74</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>6</v>
+      </c>
+      <c r="R13" s="8">
+        <v>80</v>
+      </c>
+      <c r="S13" s="8">
+        <v>2</v>
+      </c>
+      <c r="T13" s="8">
+        <v>1</v>
+      </c>
+      <c r="U13" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
@@ -1232,8 +1484,26 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P14" s="8">
+        <v>85</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>72</v>
+      </c>
+      <c r="R14" s="8">
+        <v>157</v>
+      </c>
+      <c r="S14" s="8">
+        <v>5</v>
+      </c>
+      <c r="T14" s="8">
+        <v>5</v>
+      </c>
+      <c r="U14" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
@@ -1281,8 +1551,26 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P15" s="8">
+        <v>132</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>71</v>
+      </c>
+      <c r="R15" s="8">
+        <v>203</v>
+      </c>
+      <c r="S15" s="8">
+        <v>4</v>
+      </c>
+      <c r="T15" s="8">
+        <v>5</v>
+      </c>
+      <c r="U15" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
@@ -1330,8 +1618,26 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P16" s="8">
+        <v>84</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>8</v>
+      </c>
+      <c r="R16" s="8">
+        <v>92</v>
+      </c>
+      <c r="S16" s="8">
+        <v>5</v>
+      </c>
+      <c r="T16" s="8">
+        <v>3</v>
+      </c>
+      <c r="U16" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>12</v>
       </c>
@@ -1379,8 +1685,26 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P17" s="8">
+        <v>87</v>
+      </c>
+      <c r="Q17" s="8">
+        <v>45</v>
+      </c>
+      <c r="R17" s="8">
+        <v>129</v>
+      </c>
+      <c r="S17" s="8">
+        <v>5</v>
+      </c>
+      <c r="T17" s="8">
+        <v>3</v>
+      </c>
+      <c r="U17" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
@@ -1428,8 +1752,26 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P18" s="8">
+        <v>66</v>
+      </c>
+      <c r="Q18" s="8">
+        <v>8</v>
+      </c>
+      <c r="R18" s="8">
+        <v>74</v>
+      </c>
+      <c r="S18" s="8">
+        <v>2</v>
+      </c>
+      <c r="T18" s="8">
+        <v>2</v>
+      </c>
+      <c r="U18" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>13</v>
       </c>
@@ -1477,8 +1819,26 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P19" s="8">
+        <v>99</v>
+      </c>
+      <c r="Q19" s="8">
+        <v>16</v>
+      </c>
+      <c r="R19" s="8">
+        <v>115</v>
+      </c>
+      <c r="S19" s="8">
+        <v>2</v>
+      </c>
+      <c r="T19" s="8">
+        <v>1</v>
+      </c>
+      <c r="U19" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1495,7 +1855,7 @@
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1510,7 +1870,7 @@
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F22" s="9"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added #TUS to data sheets
</commit_message>
<xml_diff>
--- a/data_analysis/task_1_2.xlsx
+++ b/data_analysis/task_1_2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4740FB18-4E8C-4ED3-80B5-F8134AF70D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1F5226-68E4-4AC6-A9AB-1475C50FFCAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23955" yWindow="3765" windowWidth="24480" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10605" yWindow="2790" windowWidth="26760" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks1&amp;2" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="39">
   <si>
     <t>Group</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Q3</t>
+  </si>
+  <si>
+    <t>#TUS</t>
   </si>
 </sst>
 </file>
@@ -555,11 +558,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U22"/>
+  <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q22" sqref="Q22"/>
+      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +570,7 @@
     <col min="1" max="21" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -590,49 +593,52 @@
         <v>19</v>
       </c>
       <c r="H1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -655,51 +661,54 @@
         <v>82</v>
       </c>
       <c r="H2" s="8">
+        <v>5</v>
+      </c>
+      <c r="I2" s="8">
         <v>10</v>
       </c>
-      <c r="I2" s="8">
-        <v>0</v>
-      </c>
       <c r="J2" s="8">
+        <v>0</v>
+      </c>
+      <c r="K2" s="8">
         <v>25</v>
       </c>
-      <c r="K2" s="8">
+      <c r="L2" s="8">
         <v>11</v>
       </c>
-      <c r="L2" s="8">
-        <f t="shared" ref="L2:L19" si="0">SUM(J2:K2)</f>
+      <c r="M2" s="8">
+        <f t="shared" ref="M2:M19" si="0">SUM(K2:L2)</f>
         <v>36</v>
       </c>
-      <c r="M2" s="8">
+      <c r="N2" s="8">
         <v>14</v>
       </c>
-      <c r="N2" s="8">
-        <v>0</v>
-      </c>
       <c r="O2" s="8">
-        <f t="shared" ref="O2:O19" si="1">SUM(M2:N2)</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="8">
+        <f t="shared" ref="P2:P19" si="1">SUM(N2:O2)</f>
         <v>14</v>
       </c>
-      <c r="P2" s="8">
+      <c r="Q2" s="8">
         <v>102</v>
       </c>
-      <c r="Q2" s="8">
+      <c r="R2" s="8">
         <v>60</v>
       </c>
-      <c r="R2" s="8">
+      <c r="S2" s="8">
         <v>162</v>
       </c>
-      <c r="S2" s="8">
-        <v>5</v>
-      </c>
       <c r="T2" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="U2" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V2" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -722,51 +731,54 @@
         <v>74</v>
       </c>
       <c r="H3" s="8">
+        <v>5</v>
+      </c>
+      <c r="I3" s="8">
         <v>10</v>
       </c>
-      <c r="I3" s="8">
+      <c r="J3" s="8">
         <v>1</v>
       </c>
-      <c r="J3" s="8">
+      <c r="K3" s="8">
         <v>24</v>
       </c>
-      <c r="K3" s="8">
+      <c r="L3" s="8">
         <v>11</v>
       </c>
-      <c r="L3" s="8">
+      <c r="M3" s="8">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="M3" s="8">
+      <c r="N3" s="8">
         <v>29</v>
       </c>
-      <c r="N3" s="8">
-        <v>0</v>
-      </c>
       <c r="O3" s="8">
+        <v>0</v>
+      </c>
+      <c r="P3" s="8">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="P3" s="8">
+      <c r="Q3" s="8">
         <v>146</v>
       </c>
-      <c r="Q3" s="8">
+      <c r="R3" s="8">
         <v>81</v>
       </c>
-      <c r="R3" s="8">
+      <c r="S3" s="8">
         <v>207</v>
       </c>
-      <c r="S3" s="8">
-        <v>3</v>
-      </c>
       <c r="T3" s="8">
         <v>3</v>
       </c>
       <c r="U3" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V3" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -789,51 +801,54 @@
         <v>73</v>
       </c>
       <c r="H4" s="8">
+        <v>5</v>
+      </c>
+      <c r="I4" s="8">
         <v>10</v>
       </c>
-      <c r="I4" s="8">
-        <v>0</v>
-      </c>
       <c r="J4" s="8">
+        <v>0</v>
+      </c>
+      <c r="K4" s="8">
         <v>25</v>
       </c>
-      <c r="K4" s="8">
+      <c r="L4" s="8">
         <v>11</v>
       </c>
-      <c r="L4" s="8">
+      <c r="M4" s="8">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="M4" s="8">
+      <c r="N4" s="8">
         <v>17</v>
       </c>
-      <c r="N4" s="8">
-        <v>0</v>
-      </c>
       <c r="O4" s="8">
+        <v>0</v>
+      </c>
+      <c r="P4" s="8">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="P4" s="8">
+      <c r="Q4" s="8">
         <v>90</v>
       </c>
-      <c r="Q4" s="8">
+      <c r="R4" s="8">
         <v>64</v>
       </c>
-      <c r="R4" s="8">
+      <c r="S4" s="8">
         <v>154</v>
       </c>
-      <c r="S4" s="8">
-        <v>4</v>
-      </c>
       <c r="T4" s="8">
+        <v>4</v>
+      </c>
+      <c r="U4" s="8">
         <v>2</v>
       </c>
-      <c r="U4" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V4" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -856,51 +871,54 @@
         <v>94.433300000000003</v>
       </c>
       <c r="H5" s="8">
+        <v>3</v>
+      </c>
+      <c r="I5" s="8">
         <v>9</v>
       </c>
-      <c r="I5" s="8">
+      <c r="J5" s="8">
         <v>1</v>
       </c>
-      <c r="J5" s="8">
+      <c r="K5" s="8">
         <v>18</v>
       </c>
-      <c r="K5" s="8">
+      <c r="L5" s="8">
         <v>10</v>
       </c>
-      <c r="L5" s="8">
+      <c r="M5" s="8">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="M5" s="8">
+      <c r="N5" s="8">
         <v>27</v>
       </c>
-      <c r="N5" s="8">
-        <v>0</v>
-      </c>
       <c r="O5" s="8">
+        <v>0</v>
+      </c>
+      <c r="P5" s="8">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="P5" s="8">
+      <c r="Q5" s="8">
         <v>121</v>
       </c>
-      <c r="Q5" s="8">
+      <c r="R5" s="8">
         <v>57</v>
       </c>
-      <c r="R5" s="8">
+      <c r="S5" s="8">
         <v>178</v>
       </c>
-      <c r="S5" s="8">
-        <v>4</v>
-      </c>
       <c r="T5" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U5" s="8">
+        <v>3</v>
+      </c>
+      <c r="V5" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -923,51 +941,54 @@
         <v>96</v>
       </c>
       <c r="H6" s="8">
+        <v>5</v>
+      </c>
+      <c r="I6" s="8">
         <v>8</v>
       </c>
-      <c r="I6" s="8">
+      <c r="J6" s="8">
         <v>1</v>
       </c>
-      <c r="J6" s="8">
+      <c r="K6" s="8">
         <v>28</v>
       </c>
-      <c r="K6" s="8">
+      <c r="L6" s="8">
         <v>16</v>
       </c>
-      <c r="L6" s="8">
+      <c r="M6" s="8">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="M6" s="8">
+      <c r="N6" s="8">
         <v>25</v>
       </c>
-      <c r="N6" s="8">
+      <c r="O6" s="8">
         <v>9</v>
       </c>
-      <c r="O6" s="8">
+      <c r="P6" s="8">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="P6" s="8">
+      <c r="Q6" s="8">
         <v>93</v>
       </c>
-      <c r="Q6" s="8">
+      <c r="R6" s="8">
         <v>102</v>
       </c>
-      <c r="R6" s="8">
+      <c r="S6" s="8">
         <v>195</v>
       </c>
-      <c r="S6" s="8">
-        <v>5</v>
-      </c>
       <c r="T6" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U6" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V6" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -990,51 +1011,54 @@
         <v>88.886600000000001</v>
       </c>
       <c r="H7" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I7" s="8">
+        <v>5</v>
+      </c>
+      <c r="J7" s="8">
         <v>9</v>
       </c>
-      <c r="J7" s="8">
+      <c r="K7" s="8">
         <v>36</v>
       </c>
-      <c r="K7" s="8">
+      <c r="L7" s="8">
         <v>16</v>
       </c>
-      <c r="L7" s="8">
+      <c r="M7" s="8">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="M7" s="8">
+      <c r="N7" s="8">
         <v>49</v>
       </c>
-      <c r="N7" s="8">
+      <c r="O7" s="8">
         <v>10</v>
       </c>
-      <c r="O7" s="8">
+      <c r="P7" s="8">
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
-      <c r="P7" s="8">
+      <c r="Q7" s="8">
         <v>164</v>
       </c>
-      <c r="Q7" s="8">
+      <c r="R7" s="8">
         <v>96</v>
       </c>
-      <c r="R7" s="8">
+      <c r="S7" s="8">
         <v>260</v>
       </c>
-      <c r="S7" s="8">
-        <v>5</v>
-      </c>
       <c r="T7" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="U7" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V7" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -1057,51 +1081,54 @@
         <v>73.55</v>
       </c>
       <c r="H8" s="8">
+        <v>5</v>
+      </c>
+      <c r="I8" s="8">
         <v>10</v>
       </c>
-      <c r="I8" s="8">
+      <c r="J8" s="8">
         <v>1</v>
       </c>
-      <c r="J8" s="8">
+      <c r="K8" s="8">
         <v>21</v>
       </c>
-      <c r="K8" s="8">
+      <c r="L8" s="8">
         <v>11</v>
       </c>
-      <c r="L8" s="8">
+      <c r="M8" s="8">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="M8" s="8">
+      <c r="N8" s="8">
         <v>20</v>
       </c>
-      <c r="N8" s="8">
-        <v>0</v>
-      </c>
       <c r="O8" s="8">
+        <v>0</v>
+      </c>
+      <c r="P8" s="8">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="P8" s="8">
+      <c r="Q8" s="8">
         <v>90</v>
       </c>
-      <c r="Q8" s="8">
+      <c r="R8" s="8">
         <v>67</v>
       </c>
-      <c r="R8" s="8">
+      <c r="S8" s="8">
         <v>157</v>
       </c>
-      <c r="S8" s="8">
-        <v>3</v>
-      </c>
       <c r="T8" s="8">
         <v>3</v>
       </c>
       <c r="U8" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V8" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
@@ -1124,51 +1151,54 @@
         <v>75</v>
       </c>
       <c r="H9" s="8">
+        <v>2</v>
+      </c>
+      <c r="I9" s="8">
         <v>12</v>
       </c>
-      <c r="I9" s="8">
+      <c r="J9" s="8">
         <v>2</v>
       </c>
-      <c r="J9" s="8">
+      <c r="K9" s="8">
         <v>16</v>
       </c>
-      <c r="K9" s="8">
+      <c r="L9" s="8">
         <v>12</v>
       </c>
-      <c r="L9" s="8">
+      <c r="M9" s="8">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="M9" s="8">
+      <c r="N9" s="8">
         <v>11</v>
       </c>
-      <c r="N9" s="8">
-        <v>0</v>
-      </c>
       <c r="O9" s="8">
+        <v>0</v>
+      </c>
+      <c r="P9" s="8">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="P9" s="8">
+      <c r="Q9" s="8">
         <v>111</v>
       </c>
-      <c r="Q9" s="8">
+      <c r="R9" s="8">
         <v>74</v>
       </c>
-      <c r="R9" s="8">
+      <c r="S9" s="8">
         <v>185</v>
       </c>
-      <c r="S9" s="8">
-        <v>4</v>
-      </c>
       <c r="T9" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U9" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="V9" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1191,51 +1221,54 @@
         <v>78.777699999999996</v>
       </c>
       <c r="H10" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I10" s="8">
         <v>0</v>
       </c>
       <c r="J10" s="8">
+        <v>0</v>
+      </c>
+      <c r="K10" s="8">
         <v>16</v>
       </c>
-      <c r="K10" s="8">
-        <v>0</v>
-      </c>
       <c r="L10" s="8">
+        <v>0</v>
+      </c>
+      <c r="M10" s="8">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="M10" s="8">
+      <c r="N10" s="8">
         <v>15</v>
       </c>
-      <c r="N10" s="8">
-        <v>0</v>
-      </c>
       <c r="O10" s="8">
+        <v>0</v>
+      </c>
+      <c r="P10" s="8">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="P10" s="8">
+      <c r="Q10" s="8">
         <v>82</v>
       </c>
-      <c r="Q10" s="8">
+      <c r="R10" s="8">
         <v>8</v>
       </c>
-      <c r="R10" s="8">
+      <c r="S10" s="8">
         <v>100</v>
       </c>
-      <c r="S10" s="8">
-        <v>4</v>
-      </c>
       <c r="T10" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U10" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V10" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1258,51 +1291,54 @@
         <v>100</v>
       </c>
       <c r="H11" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I11" s="8">
+        <v>3</v>
+      </c>
+      <c r="J11" s="8">
         <v>1</v>
       </c>
-      <c r="J11" s="8">
+      <c r="K11" s="8">
         <v>10</v>
       </c>
-      <c r="K11" s="8">
-        <v>4</v>
-      </c>
       <c r="L11" s="8">
+        <v>4</v>
+      </c>
+      <c r="M11" s="8">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="M11" s="8">
-        <v>4</v>
-      </c>
       <c r="N11" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O11" s="8">
+        <v>0</v>
+      </c>
+      <c r="P11" s="8">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="P11" s="8">
+      <c r="Q11" s="8">
         <v>86</v>
       </c>
-      <c r="Q11" s="8">
+      <c r="R11" s="8">
         <v>27</v>
       </c>
-      <c r="R11" s="8">
+      <c r="S11" s="8">
         <v>113</v>
-      </c>
-      <c r="S11" s="8">
-        <v>2</v>
       </c>
       <c r="T11" s="8">
         <v>2</v>
       </c>
       <c r="U11" s="8">
+        <v>2</v>
+      </c>
+      <c r="V11" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
@@ -1325,51 +1361,54 @@
         <v>69.333299999999994</v>
       </c>
       <c r="H12" s="8">
+        <v>5</v>
+      </c>
+      <c r="I12" s="8">
         <v>7</v>
       </c>
-      <c r="I12" s="8">
+      <c r="J12" s="8">
         <v>1</v>
       </c>
-      <c r="J12" s="8">
+      <c r="K12" s="8">
         <v>16</v>
       </c>
-      <c r="K12" s="8">
+      <c r="L12" s="8">
         <v>8</v>
       </c>
-      <c r="L12" s="8">
+      <c r="M12" s="8">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="M12" s="8">
+      <c r="N12" s="8">
         <v>17</v>
       </c>
-      <c r="N12" s="8">
-        <v>0</v>
-      </c>
       <c r="O12" s="8">
+        <v>0</v>
+      </c>
+      <c r="P12" s="8">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="P12" s="8">
+      <c r="Q12" s="8">
         <v>90</v>
       </c>
-      <c r="Q12" s="8">
+      <c r="R12" s="8">
         <v>45</v>
       </c>
-      <c r="R12" s="8">
+      <c r="S12" s="8">
         <v>135</v>
       </c>
-      <c r="S12" s="8">
-        <v>5</v>
-      </c>
       <c r="T12" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U12" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V12" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
@@ -1398,45 +1437,48 @@
         <v>0</v>
       </c>
       <c r="J13" s="8">
+        <v>0</v>
+      </c>
+      <c r="K13" s="8">
         <v>9</v>
       </c>
-      <c r="K13" s="8">
-        <v>0</v>
-      </c>
       <c r="L13" s="8">
+        <v>0</v>
+      </c>
+      <c r="M13" s="8">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="M13" s="8">
+      <c r="N13" s="8">
         <v>2</v>
       </c>
-      <c r="N13" s="8">
-        <v>0</v>
-      </c>
       <c r="O13" s="8">
+        <v>0</v>
+      </c>
+      <c r="P13" s="8">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="P13" s="8">
+      <c r="Q13" s="8">
         <v>74</v>
       </c>
-      <c r="Q13" s="8">
+      <c r="R13" s="8">
         <v>6</v>
       </c>
-      <c r="R13" s="8">
+      <c r="S13" s="8">
         <v>80</v>
       </c>
-      <c r="S13" s="8">
+      <c r="T13" s="8">
         <v>2</v>
-      </c>
-      <c r="T13" s="8">
-        <v>1</v>
       </c>
       <c r="U13" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V13" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
@@ -1459,51 +1501,54 @@
         <v>82</v>
       </c>
       <c r="H14" s="8">
+        <v>5</v>
+      </c>
+      <c r="I14" s="8">
         <v>12</v>
       </c>
-      <c r="I14" s="8">
-        <v>0</v>
-      </c>
       <c r="J14" s="8">
+        <v>0</v>
+      </c>
+      <c r="K14" s="8">
         <v>16</v>
       </c>
-      <c r="K14" s="8">
+      <c r="L14" s="8">
         <v>13</v>
       </c>
-      <c r="L14" s="8">
+      <c r="M14" s="8">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="M14" s="8">
+      <c r="N14" s="8">
         <v>14</v>
       </c>
-      <c r="N14" s="8">
-        <v>0</v>
-      </c>
       <c r="O14" s="8">
+        <v>0</v>
+      </c>
+      <c r="P14" s="8">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="P14" s="8">
+      <c r="Q14" s="8">
         <v>85</v>
       </c>
-      <c r="Q14" s="8">
+      <c r="R14" s="8">
         <v>72</v>
       </c>
-      <c r="R14" s="8">
+      <c r="S14" s="8">
         <v>157</v>
       </c>
-      <c r="S14" s="8">
-        <v>5</v>
-      </c>
       <c r="T14" s="8">
         <v>5</v>
       </c>
       <c r="U14" s="8">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V14" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
@@ -1526,51 +1571,54 @@
         <v>100</v>
       </c>
       <c r="H15" s="8">
+        <v>5</v>
+      </c>
+      <c r="I15" s="8">
         <v>13</v>
       </c>
-      <c r="I15" s="8">
+      <c r="J15" s="8">
         <v>2</v>
       </c>
-      <c r="J15" s="8">
+      <c r="K15" s="8">
         <v>19</v>
       </c>
-      <c r="K15" s="8">
+      <c r="L15" s="8">
         <v>14</v>
       </c>
-      <c r="L15" s="8">
+      <c r="M15" s="8">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="M15" s="8">
+      <c r="N15" s="8">
         <v>40</v>
       </c>
-      <c r="N15" s="8">
-        <v>0</v>
-      </c>
       <c r="O15" s="8">
+        <v>0</v>
+      </c>
+      <c r="P15" s="8">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="P15" s="8">
+      <c r="Q15" s="8">
         <v>132</v>
       </c>
-      <c r="Q15" s="8">
+      <c r="R15" s="8">
         <v>71</v>
       </c>
-      <c r="R15" s="8">
+      <c r="S15" s="8">
         <v>203</v>
       </c>
-      <c r="S15" s="8">
-        <v>4</v>
-      </c>
       <c r="T15" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U15" s="8">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V15" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
@@ -1593,51 +1641,54 @@
         <v>81.111099999999993</v>
       </c>
       <c r="H16" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I16" s="8">
         <v>0</v>
       </c>
       <c r="J16" s="8">
+        <v>0</v>
+      </c>
+      <c r="K16" s="8">
         <v>18</v>
       </c>
-      <c r="K16" s="8">
-        <v>0</v>
-      </c>
       <c r="L16" s="8">
+        <v>0</v>
+      </c>
+      <c r="M16" s="8">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="M16" s="8">
+      <c r="N16" s="8">
         <v>15</v>
       </c>
-      <c r="N16" s="8">
-        <v>0</v>
-      </c>
       <c r="O16" s="8">
+        <v>0</v>
+      </c>
+      <c r="P16" s="8">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="P16" s="8">
+      <c r="Q16" s="8">
         <v>84</v>
       </c>
-      <c r="Q16" s="8">
+      <c r="R16" s="8">
         <v>8</v>
       </c>
-      <c r="R16" s="8">
+      <c r="S16" s="8">
         <v>92</v>
       </c>
-      <c r="S16" s="8">
-        <v>5</v>
-      </c>
       <c r="T16" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="U16" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V16" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>12</v>
       </c>
@@ -1660,51 +1711,54 @@
         <v>100</v>
       </c>
       <c r="H17" s="8">
+        <v>2</v>
+      </c>
+      <c r="I17" s="8">
         <v>8</v>
       </c>
-      <c r="I17" s="8">
-        <v>0</v>
-      </c>
       <c r="J17" s="8">
+        <v>0</v>
+      </c>
+      <c r="K17" s="8">
         <v>10</v>
       </c>
-      <c r="K17" s="8">
+      <c r="L17" s="8">
         <v>8</v>
       </c>
-      <c r="L17" s="8">
+      <c r="M17" s="8">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="M17" s="8">
-        <v>4</v>
-      </c>
       <c r="N17" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O17" s="8">
+        <v>0</v>
+      </c>
+      <c r="P17" s="8">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="P17" s="8">
+      <c r="Q17" s="8">
         <v>87</v>
       </c>
-      <c r="Q17" s="8">
+      <c r="R17" s="8">
         <v>45</v>
       </c>
-      <c r="R17" s="8">
+      <c r="S17" s="8">
         <v>129</v>
       </c>
-      <c r="S17" s="8">
-        <v>5</v>
-      </c>
       <c r="T17" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="U17" s="8">
+        <v>3</v>
+      </c>
+      <c r="V17" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
@@ -1727,51 +1781,54 @@
         <v>65.555499999999995</v>
       </c>
       <c r="H18" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I18" s="8">
         <v>0</v>
       </c>
       <c r="J18" s="8">
+        <v>0</v>
+      </c>
+      <c r="K18" s="8">
         <v>12</v>
       </c>
-      <c r="K18" s="8">
-        <v>0</v>
-      </c>
       <c r="L18" s="8">
+        <v>0</v>
+      </c>
+      <c r="M18" s="8">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="M18" s="8">
+      <c r="N18" s="8">
         <v>9</v>
       </c>
-      <c r="N18" s="8">
-        <v>0</v>
-      </c>
       <c r="O18" s="8">
+        <v>0</v>
+      </c>
+      <c r="P18" s="8">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="P18" s="8">
+      <c r="Q18" s="8">
         <v>66</v>
       </c>
-      <c r="Q18" s="8">
+      <c r="R18" s="8">
         <v>8</v>
       </c>
-      <c r="R18" s="8">
+      <c r="S18" s="8">
         <v>74</v>
-      </c>
-      <c r="S18" s="8">
-        <v>2</v>
       </c>
       <c r="T18" s="8">
         <v>2</v>
       </c>
       <c r="U18" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="V18" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>13</v>
       </c>
@@ -1797,48 +1854,51 @@
         <v>3</v>
       </c>
       <c r="I19" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J19" s="8">
+        <v>0</v>
+      </c>
+      <c r="K19" s="8">
         <v>12</v>
       </c>
-      <c r="K19" s="8">
-        <v>3</v>
-      </c>
       <c r="L19" s="8">
+        <v>3</v>
+      </c>
+      <c r="M19" s="8">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="M19" s="8">
+      <c r="N19" s="8">
         <v>14</v>
       </c>
-      <c r="N19" s="8">
-        <v>0</v>
-      </c>
       <c r="O19" s="8">
+        <v>0</v>
+      </c>
+      <c r="P19" s="8">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="P19" s="8">
+      <c r="Q19" s="8">
         <v>99</v>
       </c>
-      <c r="Q19" s="8">
+      <c r="R19" s="8">
         <v>16</v>
       </c>
-      <c r="R19" s="8">
+      <c r="S19" s="8">
         <v>115</v>
       </c>
-      <c r="S19" s="8">
+      <c r="T19" s="8">
         <v>2</v>
       </c>
-      <c r="T19" s="8">
+      <c r="U19" s="8">
         <v>1</v>
       </c>
-      <c r="U19" s="8">
+      <c r="V19" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1855,7 +1915,7 @@
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1870,14 +1930,11 @@
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F22" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="L2:L19" formulaRange="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>